<commit_message>
- Added blocking to the simulation logic
</commit_message>
<xml_diff>
--- a/Statistical_Analysis.xlsx
+++ b/Statistical_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e542966a5cb5940/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e542966a5cb5940/Desktop/SYSC 4005 A/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="11_F25DC773A252ABDACC10488379DF768E5ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C541975-C47A-4A9F-B5BC-540A37BD745E}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="11_F25DC773A252ABDACC10488379DF768E5ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF8C200-0648-4EC6-B12D-978736D65FCC}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="12318" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inspector1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <definedName name="_xlchart.v1.1" hidden="1">Inspector2_2!$A$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">'Workstation 3'!$A$2:$A$301</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Kolmogorov!$A$2:$A$151</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Kolmogorov!$A$2:$A$151</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Inspector2_2!$A$2:$A$301</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Inspector2_3!$A$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Inspector2_3!$A$2:$A$301</definedName>
@@ -13192,7 +13191,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -20507,7 +20506,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7225665" y="180975"/>
+              <a:off x="11344275" y="180975"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -20590,7 +20589,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7901946" y="226695"/>
+              <a:off x="10050786" y="226695"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -20709,7 +20708,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8157210" y="127635"/>
+              <a:off x="10363200" y="127635"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -20828,7 +20827,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6777996" y="302895"/>
+              <a:off x="8465826" y="302895"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -21185,8 +21184,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1866900" y="1252537"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="1868805" y="1263967"/>
+              <a:ext cx="4585335" cy="2773680"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -21217,6 +21216,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21485,7 +21488,7 @@
   <dimension ref="A1:J307"/>
   <sheetViews>
     <sheetView topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -27094,7 +27097,7 @@
         <v>95.842066637357945</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -27102,8 +27105,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>10.357909999999999</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>9.6544573181269203E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -27112,7 +27119,7 @@
         <v>9.7898961504889286</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>
@@ -27135,8 +27142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F35057-6B93-4BE2-873C-A6C7C96A6357}">
   <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -32743,7 +32750,7 @@
         <v>215.64430796721268</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -32751,8 +32758,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>15.536903333333338</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>6.4362889988159352E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -32761,7 +32772,7 @@
         <v>14.684832582198977</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>
@@ -32784,7 +32795,7 @@
   <dimension ref="A1:J307"/>
   <sheetViews>
     <sheetView topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38390,7 +38401,7 @@
         <v>394.38618728841692</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -38398,8 +38409,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>20.632756666666669</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>4.8466621118813169E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -38408,7 +38423,7 @@
         <v>19.859158775950629</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>
@@ -38431,7 +38446,7 @@
   <dimension ref="A1:J307"/>
   <sheetViews>
     <sheetView topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -44037,7 +44052,7 @@
         <v>22.62537499303232</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -44045,8 +44060,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>4.6044166666666664</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>0.21718277740575173</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -44055,7 +44074,7 @@
         <v>4.756613815839196</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>
@@ -44078,7 +44097,7 @@
   <dimension ref="A1:J307"/>
   <sheetViews>
     <sheetView topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -49683,7 +49702,7 @@
         <v>140.33756404544027</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -49691,8 +49710,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>11.092606666666669</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>9.0150136036555265E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -49701,7 +49724,7 @@
         <v>11.846415662361348</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>
@@ -49723,8 +49746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE48D7E8-CB7F-4A53-8F96-69233EAAEC76}">
   <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -55330,7 +55353,7 @@
         <v>74.825445802943051</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" t="s">
         <v>7</v>
       </c>
@@ -55338,8 +55361,12 @@
         <f xml:space="preserve"> SUM(A2:A301) / 300</f>
         <v>8.7955800000000046</v>
       </c>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D305">
+        <f xml:space="preserve"> 1 / C305</f>
+        <v>0.11369346876499327</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" t="s">
         <v>8</v>
       </c>
@@ -55348,7 +55375,7 @@
         <v>8.6501702759508188</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" t="s">
         <v>11</v>
       </c>

</xml_diff>